<commit_message>
📖 docs: Add manual testing metrics documentation
Uploaded detailed test metrics for manual testing, including test execution results, pass/fail counts, coverage statistics, and defect tracking. Provides visibility into testing outcomes and supports evaluation of project quality and readiness.
</commit_message>
<xml_diff>
--- a/Test Cases/KaBuM Web Testing.xlsx
+++ b/Test Cases/KaBuM Web Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SUDIPTA\Programming\SQA\KaBuM-Web-App-Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7502D88-7884-47B9-9A99-CD28F6592908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D237FC-539E-4B24-B3B4-7CABD295023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,6 +182,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Before Click Continue</t>
     </r>
@@ -189,6 +190,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -199,6 +201,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>After Click Continue</t>
     </r>
@@ -247,6 +250,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Before Click Continue</t>
     </r>
@@ -254,6 +258,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -264,6 +269,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>After Click Continue</t>
     </r>
@@ -306,6 +312,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Before Click Continue</t>
     </r>
@@ -313,6 +320,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -323,6 +331,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>After Click Continue</t>
     </r>
@@ -360,6 +369,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Before Click Continue</t>
     </r>
@@ -367,6 +377,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -377,6 +388,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>After Click Continue</t>
     </r>
@@ -513,6 +525,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>image1</t>
     </r>
@@ -522,6 +535,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (OK)
 </t>
@@ -532,6 +546,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>image2</t>
     </r>
@@ -541,6 +556,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (Fault)</t>
     </r>
@@ -766,7 +782,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -778,26 +794,31 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="17"/>
       <color rgb="FFFF9900"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -805,46 +826,60 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1076,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1168,6 +1203,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1180,29 +1239,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1426,7 +1467,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1448,10 +1489,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="44"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1472,10 +1513,10 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="32"/>
+      <c r="N1" s="40"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
@@ -1490,21 +1531,21 @@
       <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="34" t="s">
         <v>162</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="41">
+      <c r="G2" s="34">
         <v>45893</v>
       </c>
       <c r="H2" s="4"/>
@@ -1512,7 +1553,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="31" t="s">
         <v>8</v>
       </c>
       <c r="N2" s="9">
@@ -1533,10 +1574,10 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
         <v>10</v>
@@ -1555,7 +1596,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="36" t="s">
+      <c r="M3" s="32" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="9">
@@ -1576,10 +1617,10 @@
       <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
@@ -1617,23 +1658,23 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="32"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="42" t="s">
+      <c r="M5" s="35" t="s">
         <v>20</v>
       </c>
       <c r="N5" s="9">
@@ -1742,7 +1783,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +1818,7 @@
         <v>46</v>
       </c>
       <c r="L8" s="20"/>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="36" t="s">
         <v>47</v>
       </c>
       <c r="N8" s="20"/>
@@ -1794,7 +1835,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>48</v>
       </c>
@@ -1829,7 +1870,7 @@
         <v>46</v>
       </c>
       <c r="L9" s="20"/>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="37" t="s">
         <v>47</v>
       </c>
       <c r="N9" s="20"/>
@@ -1846,7 +1887,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>55</v>
       </c>
@@ -1881,7 +1922,7 @@
         <v>46</v>
       </c>
       <c r="L10" s="20"/>
-      <c r="M10" s="38" t="s">
+      <c r="M10" s="37" t="s">
         <v>47</v>
       </c>
       <c r="N10" s="20"/>
@@ -1898,7 +1939,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="229.5" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>62</v>
       </c>
@@ -1950,7 +1991,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>69</v>
       </c>
@@ -2089,7 +2130,7 @@
         <v>88</v>
       </c>
       <c r="L14" s="7"/>
-      <c r="M14" s="38" t="s">
+      <c r="M14" s="37" t="s">
         <v>47</v>
       </c>
       <c r="N14" s="7"/>
@@ -2106,7 +2147,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:26" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>89</v>
       </c>
@@ -2141,7 +2182,7 @@
         <v>88</v>
       </c>
       <c r="L15" s="5"/>
-      <c r="M15" s="38" t="s">
+      <c r="M15" s="37" t="s">
         <v>47</v>
       </c>
       <c r="N15" s="7"/>
@@ -2158,7 +2199,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="153" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>93</v>
       </c>
@@ -2193,7 +2234,7 @@
         <v>88</v>
       </c>
       <c r="L16" s="20"/>
-      <c r="M16" s="40" t="s">
+      <c r="M16" s="38" t="s">
         <v>68</v>
       </c>
       <c r="N16" s="7"/>
@@ -2210,7 +2251,7 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
     </row>
-    <row r="17" spans="1:26" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>99</v>
       </c>
@@ -2245,7 +2286,7 @@
         <v>88</v>
       </c>
       <c r="L17" s="20"/>
-      <c r="M17" s="38" t="s">
+      <c r="M17" s="37" t="s">
         <v>47</v>
       </c>
       <c r="N17" s="7"/>
@@ -2262,7 +2303,7 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>107</v>
       </c>
@@ -2297,7 +2338,7 @@
         <v>75</v>
       </c>
       <c r="L18" s="20"/>
-      <c r="M18" s="38" t="s">
+      <c r="M18" s="37" t="s">
         <v>47</v>
       </c>
       <c r="N18" s="7"/>
@@ -2314,7 +2355,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" spans="1:26" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>114</v>
       </c>
@@ -2349,7 +2390,7 @@
         <v>123</v>
       </c>
       <c r="L19" s="20"/>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="38" t="s">
         <v>68</v>
       </c>
       <c r="N19" s="7"/>
@@ -2383,7 +2424,7 @@
         <v>123</v>
       </c>
       <c r="L20" s="20"/>
-      <c r="M20" s="39"/>
+      <c r="M20" s="33"/>
       <c r="N20" s="7"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -2415,7 +2456,7 @@
         <v>123</v>
       </c>
       <c r="L21" s="7"/>
-      <c r="M21" s="39"/>
+      <c r="M21" s="33"/>
       <c r="N21" s="7"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
@@ -2447,7 +2488,7 @@
         <v>123</v>
       </c>
       <c r="L22" s="7"/>
-      <c r="M22" s="39"/>
+      <c r="M22" s="33"/>
       <c r="N22" s="7"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -2479,7 +2520,7 @@
         <v>123</v>
       </c>
       <c r="L23" s="7"/>
-      <c r="M23" s="39"/>
+      <c r="M23" s="33"/>
       <c r="N23" s="7"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -2511,7 +2552,7 @@
         <v>123</v>
       </c>
       <c r="L24" s="7"/>
-      <c r="M24" s="39"/>
+      <c r="M24" s="33"/>
       <c r="N24" s="7"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -2543,7 +2584,7 @@
         <v>123</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="39"/>
+      <c r="M25" s="33"/>
       <c r="N25" s="7"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -2575,7 +2616,7 @@
         <v>123</v>
       </c>
       <c r="L26" s="7"/>
-      <c r="M26" s="39"/>
+      <c r="M26" s="33"/>
       <c r="N26" s="7"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -2607,7 +2648,7 @@
         <v>123</v>
       </c>
       <c r="L27" s="7"/>
-      <c r="M27" s="39"/>
+      <c r="M27" s="33"/>
       <c r="N27" s="7"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -2639,7 +2680,7 @@
         <v>123</v>
       </c>
       <c r="L28" s="7"/>
-      <c r="M28" s="39"/>
+      <c r="M28" s="33"/>
       <c r="N28" s="7"/>
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
@@ -2671,7 +2712,7 @@
         <v>123</v>
       </c>
       <c r="L29" s="7"/>
-      <c r="M29" s="39"/>
+      <c r="M29" s="33"/>
       <c r="N29" s="7"/>
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
@@ -2703,7 +2744,7 @@
         <v>123</v>
       </c>
       <c r="L30" s="7"/>
-      <c r="M30" s="39"/>
+      <c r="M30" s="33"/>
       <c r="N30" s="7"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
@@ -2735,7 +2776,7 @@
         <v>123</v>
       </c>
       <c r="L31" s="7"/>
-      <c r="M31" s="39"/>
+      <c r="M31" s="33"/>
       <c r="N31" s="7"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
@@ -2767,7 +2808,7 @@
         <v>123</v>
       </c>
       <c r="L32" s="7"/>
-      <c r="M32" s="39"/>
+      <c r="M32" s="33"/>
       <c r="N32" s="7"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
@@ -2799,7 +2840,7 @@
         <v>123</v>
       </c>
       <c r="L33" s="7"/>
-      <c r="M33" s="39"/>
+      <c r="M33" s="33"/>
       <c r="N33" s="7"/>
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
@@ -2831,7 +2872,7 @@
         <v>123</v>
       </c>
       <c r="L34" s="7"/>
-      <c r="M34" s="39"/>
+      <c r="M34" s="33"/>
       <c r="N34" s="7"/>
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
@@ -2863,7 +2904,7 @@
         <v>123</v>
       </c>
       <c r="L35" s="7"/>
-      <c r="M35" s="39"/>
+      <c r="M35" s="33"/>
       <c r="N35" s="7"/>
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
@@ -2895,7 +2936,7 @@
         <v>123</v>
       </c>
       <c r="L36" s="7"/>
-      <c r="M36" s="39"/>
+      <c r="M36" s="33"/>
       <c r="N36" s="7"/>
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
@@ -2927,7 +2968,7 @@
         <v>123</v>
       </c>
       <c r="L37" s="7"/>
-      <c r="M37" s="39"/>
+      <c r="M37" s="33"/>
       <c r="N37" s="7"/>
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
@@ -2959,7 +3000,7 @@
         <v>123</v>
       </c>
       <c r="L38" s="7"/>
-      <c r="M38" s="39"/>
+      <c r="M38" s="33"/>
       <c r="N38" s="7"/>
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
@@ -2991,7 +3032,7 @@
         <v>123</v>
       </c>
       <c r="L39" s="7"/>
-      <c r="M39" s="39"/>
+      <c r="M39" s="33"/>
       <c r="N39" s="7"/>
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
@@ -3023,7 +3064,7 @@
         <v>123</v>
       </c>
       <c r="L40" s="7"/>
-      <c r="M40" s="39"/>
+      <c r="M40" s="33"/>
       <c r="N40" s="7"/>
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
@@ -3055,7 +3096,7 @@
         <v>123</v>
       </c>
       <c r="L41" s="7"/>
-      <c r="M41" s="39"/>
+      <c r="M41" s="33"/>
       <c r="N41" s="7"/>
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
@@ -3087,7 +3128,7 @@
         <v>123</v>
       </c>
       <c r="L42" s="7"/>
-      <c r="M42" s="39"/>
+      <c r="M42" s="33"/>
       <c r="N42" s="7"/>
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
@@ -3119,7 +3160,7 @@
         <v>123</v>
       </c>
       <c r="L43" s="7"/>
-      <c r="M43" s="39"/>
+      <c r="M43" s="33"/>
       <c r="N43" s="7"/>
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
@@ -3151,7 +3192,7 @@
         <v>123</v>
       </c>
       <c r="L44" s="7"/>
-      <c r="M44" s="39"/>
+      <c r="M44" s="33"/>
       <c r="N44" s="7"/>
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
@@ -3183,7 +3224,7 @@
         <v>123</v>
       </c>
       <c r="L45" s="7"/>
-      <c r="M45" s="39"/>
+      <c r="M45" s="33"/>
       <c r="N45" s="7"/>
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
@@ -3215,7 +3256,7 @@
         <v>123</v>
       </c>
       <c r="L46" s="7"/>
-      <c r="M46" s="39"/>
+      <c r="M46" s="33"/>
       <c r="N46" s="7"/>
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
@@ -3247,7 +3288,7 @@
         <v>123</v>
       </c>
       <c r="L47" s="7"/>
-      <c r="M47" s="39"/>
+      <c r="M47" s="33"/>
       <c r="N47" s="7"/>
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
@@ -3279,7 +3320,7 @@
         <v>123</v>
       </c>
       <c r="L48" s="7"/>
-      <c r="M48" s="39"/>
+      <c r="M48" s="33"/>
       <c r="N48" s="7"/>
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
@@ -3311,7 +3352,7 @@
         <v>123</v>
       </c>
       <c r="L49" s="7"/>
-      <c r="M49" s="39"/>
+      <c r="M49" s="33"/>
       <c r="N49" s="7"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
@@ -3343,7 +3384,7 @@
         <v>123</v>
       </c>
       <c r="L50" s="7"/>
-      <c r="M50" s="39"/>
+      <c r="M50" s="33"/>
       <c r="N50" s="7"/>
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
@@ -3375,7 +3416,7 @@
         <v>123</v>
       </c>
       <c r="L51" s="7"/>
-      <c r="M51" s="39"/>
+      <c r="M51" s="33"/>
       <c r="N51" s="7"/>
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
@@ -3407,7 +3448,7 @@
         <v>123</v>
       </c>
       <c r="L52" s="7"/>
-      <c r="M52" s="39"/>
+      <c r="M52" s="33"/>
       <c r="N52" s="7"/>
       <c r="O52" s="6"/>
       <c r="P52" s="6"/>
@@ -3439,7 +3480,7 @@
         <v>123</v>
       </c>
       <c r="L53" s="7"/>
-      <c r="M53" s="39"/>
+      <c r="M53" s="33"/>
       <c r="N53" s="7"/>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
@@ -3471,7 +3512,7 @@
         <v>123</v>
       </c>
       <c r="L54" s="7"/>
-      <c r="M54" s="39"/>
+      <c r="M54" s="33"/>
       <c r="N54" s="7"/>
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
@@ -3503,7 +3544,7 @@
         <v>123</v>
       </c>
       <c r="L55" s="7"/>
-      <c r="M55" s="39"/>
+      <c r="M55" s="33"/>
       <c r="N55" s="7"/>
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
@@ -3535,7 +3576,7 @@
         <v>123</v>
       </c>
       <c r="L56" s="7"/>
-      <c r="M56" s="39"/>
+      <c r="M56" s="33"/>
       <c r="N56" s="7"/>
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
@@ -3567,7 +3608,7 @@
         <v>123</v>
       </c>
       <c r="L57" s="7"/>
-      <c r="M57" s="39"/>
+      <c r="M57" s="33"/>
       <c r="N57" s="7"/>
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>

</xml_diff>